<commit_message>
Declaration variable in test cases
</commit_message>
<xml_diff>
--- a/LoginResults.xlsx
+++ b/LoginResults.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hasil Login" r:id="rId3" sheetId="1"/>
+    <sheet name="Login Result" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -20,7 +20,7 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Hasil</t>
+    <t>Result</t>
   </si>
   <si>
     <t>user1</t>

</xml_diff>